<commit_message>
tunning excel download, rename 'boot'-> 'bootNotification'
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -490,7 +490,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>20220603135549924_boot</t>
+          <t>20220603170334598_boot</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -500,7 +500,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>boot</t>
+          <t>bootNotification</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>{'status': 'Accepted', 'currentTime': '2022-06-03T04:55:47Z', 'interval': 300}</t>
+          <t>{'status': 'Accepted', 'currentTime': '2022-06-03T08:03:32Z', 'interval': 300}</t>
         </is>
       </c>
     </row>
@@ -522,7 +522,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20220603135549924_boot</t>
+          <t>20220603170334598_boot</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -537,7 +537,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>{'connectorId': '01', 'errorCode': None, 'info': [{'reason': None, 'cpv': 100, 'rv': 11}], 'status': 'Available', 'timestamp': '2022-06-03T13:55:51Z', 'vendorErrorCode': '', 'vendorId': 'LGE'}</t>
+          <t>{'connectorId': '01', 'errorCode': None, 'info': [{'reason': None, 'cpv': 100, 'rv': 11}], 'status': 'Available', 'timestamp': '2022-06-03T17:03:35Z', 'vendorErrorCode': '', 'vendorId': 'LGE'}</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -559,12 +559,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>20220603135552197_card</t>
+          <t>20220603170336787_card</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NoData</t>
+          <t>ServerError</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -579,7 +579,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>{'idTagInfo': {'status': 'NoData', 'expiryDate': '2022-06-03T04:55:50Z'}}</t>
+          <t>&lt;Response [500]&gt;</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>20220603135552197_card</t>
+          <t>20220603170336787_card</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>{'connectorId': '01', 'errorCode': None, 'info': [{'reason': None, 'cpv': 100, 'rv': 11}], 'status': 'Preparing', 'timestamp': '2022-06-03T13:55:53Z', 'vendorErrorCode': '', 'vendorId': 'LGE'}</t>
+          <t>{'connectorId': '01', 'errorCode': None, 'info': [{'reason': None, 'cpv': 100, 'rv': 11}], 'status': 'Preparing', 'timestamp': '2022-06-03T17:03:37Z', 'vendorErrorCode': '', 'vendorId': 'LGE'}</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>20220603135552197_card</t>
+          <t>20220603170336787_card</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -648,7 +648,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>{'venderId': 'LG', 'messageId': 'Tariff', 'data': {'connectorId': '01', 'idTag': '1010202030306060', 'timestamp': '2022-06-03T13:55:54Z'}}</t>
+          <t>{'venderId': 'LG', 'messageId': 'Tariff', 'data': {'connectorId': '01', 'idTag': '3333222233334444', 'timestamp': '2022-06-03T17:03:38Z'}}</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -670,7 +670,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>20220603135552197_card</t>
+          <t>20220603170336787_card</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>{'idTag': '1111222233336666', 'connectorId': '01', 'meterStart': None, 'timestamp': '2022-06-03T13:55:55Z'}</t>
+          <t>{'idTag': '1111222233336666', 'connectorId': '01', 'meterStart': None, 'timestamp': '2022-06-03T17:03:40Z'}</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -707,7 +707,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>20220603135552197_card</t>
+          <t>20220603170336787_card</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -722,7 +722,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>{'connectorId': '01', 'errorCode': None, 'info': [{'reason': None, 'cpv': 100, 'rv': 11}], 'status': 'Charging', 'timestamp': '2022-06-03T13:55:56Z', 'vendorErrorCode': '', 'vendorId': 'LGE'}</t>
+          <t>{'connectorId': '01', 'errorCode': None, 'info': [{'reason': None, 'cpv': 100, 'rv': 11}], 'status': 'Charging', 'timestamp': '2022-06-03T17:03:41Z', 'vendorErrorCode': '', 'vendorId': 'LGE'}</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -744,7 +744,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>20220603135552197_card</t>
+          <t>20220603170336787_card</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -759,7 +759,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>{'connectorId': '01', 'transactionId': None, 'meterValue': [{'timestamp': '2022-06-03T13:55:57Z', 'sampledValue': [{'measurand': 'Current.Import', 'phase': 'L1', 'unit': 'A', 'value': '23.5'}, {'measurand': 'Voltage', 'phase': 'L1', 'unit': 'V', 'value': '219.9'}, {'measurand': 'Energy.Active.Import.Register', 'unit': 'Wh', 'value': '1000.2'}, {'measurand': 'SoC', 'unit': '%', 'value': '10'}, {'measurand': 'Power.Active.Import', 'unit': 'W', 'value': '-0.0'}]}]}</t>
+          <t>{'connectorId': '01', 'transactionId': None, 'meterValue': [{'timestamp': '2022-06-03T17:03:42Z', 'sampledValue': [{'measurand': 'Current.Import', 'phase': 'L1', 'unit': 'A', 'value': '24.9'}, {'measurand': 'Voltage', 'phase': 'L1', 'unit': 'V', 'value': '220.3'}, {'measurand': 'Energy.Active.Import.Register', 'unit': 'Wh', 'value': '999.8'}, {'measurand': 'SoC', 'unit': '%', 'value': '10'}, {'measurand': 'Power.Active.Import', 'unit': 'W', 'value': '1.0'}]}]}</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -781,12 +781,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>20220603135552197_card</t>
+          <t>20220603170336787_card</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Accepted</t>
+          <t>ServerError</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -796,12 +796,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>{'idTag': '3333222233334444', 'meterStop': -0.004792434873548412, 'reason': 'Finished', 'timestamp': '2022-06-03T13:55:58Z', 'transactionId': None, 'transactionData': [{'timestamp': '2022-06-03T13:55:58Z', 'sampledValue': [{'measurand': '01', 'phase': '01', 'unit': '01', 'value': '01'}, {'measurand': '01', 'phase': '01', 'unit': '01', 'value': '01'}]}]}</t>
+          <t>{'idTag': '5555222233334444', 'meterStop': 0.9795552337100024, 'reason': 'Finished', 'timestamp': '2022-06-03T17:03:43Z', 'transactionId': None, 'transactionData': [{'timestamp': '2022-06-03T17:03:43Z', 'sampledValue': [{'measurand': '01', 'phase': '01', 'unit': '01', 'value': '01'}, {'measurand': '01', 'phase': '01', 'unit': '01', 'value': '01'}]}]}</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>{'idTagInfo': {'status': 'Accepted', 'expiryDate': '2022-06-03T04:55:56Z'}, 'transactionId': '123123123'}</t>
+          <t>&lt;Response [500]&gt;</t>
         </is>
       </c>
     </row>
@@ -818,7 +818,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>20220603135552197_card</t>
+          <t>20220603170336787_card</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>{'connectorId': '01', 'errorCode': None, 'info': [{'reason': None, 'cpv': 100, 'rv': 11}], 'status': 'Finishing', 'timestamp': '2022-06-03T13:55:59Z', 'vendorErrorCode': '', 'vendorId': 'LGE'}</t>
+          <t>{'connectorId': '01', 'errorCode': None, 'info': [{'reason': None, 'cpv': 100, 'rv': 11}], 'status': 'Finishing', 'timestamp': '2022-06-03T17:03:44Z', 'vendorErrorCode': '', 'vendorId': 'LGE'}</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -855,7 +855,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>20220603135552197_card</t>
+          <t>20220603170336787_card</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -870,7 +870,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>{'connectorId': '01', 'errorCode': None, 'info': [{'reason': None, 'cpv': 100, 'rv': 11}], 'status': 'Available', 'timestamp': '2022-06-03T13:56:00Z', 'vendorErrorCode': '', 'vendorId': 'LGE'}</t>
+          <t>{'connectorId': '01', 'errorCode': None, 'info': [{'reason': None, 'cpv': 100, 'rv': 11}], 'status': 'Available', 'timestamp': '2022-06-03T17:03:45Z', 'vendorErrorCode': '', 'vendorId': 'LGE'}</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -892,7 +892,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>20220603135606373_heartbeat</t>
+          <t>20220603170354051_heartbeat</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">

</xml_diff>